<commit_message>
update README + quickstart + installation instructions
</commit_message>
<xml_diff>
--- a/mobility/data/insee/esane/shops_turnover.xlsx
+++ b/mobility/data/insee/esane/shops_turnover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauchota\Documents\repo_mobility\mobility\data\insee\esane\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\mobility_oss\mobility\data\insee\esane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F54F8DE5-2D05-4253-987D-63004BDB5097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF0689A-254F-4FB1-B212-3FB869AE7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9228" yWindow="5316" windowWidth="17280" windowHeight="8964" xr2:uid="{23ED7F08-657E-4889-BF84-26D96ADA39E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{23ED7F08-657E-4889-BF84-26D96ADA39E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>naf_id</t>
   </si>
@@ -79,15 +79,22 @@
   </si>
   <si>
     <t>sqm_pshop</t>
+  </si>
+  <si>
+    <t>n_fte_jobs</t>
+  </si>
+  <si>
+    <t>turnover_per_employee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -126,12 +133,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -151,9 +161,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,7 +201,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -297,7 +307,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D08904-E6CE-46E2-99CC-DE50532FF5D3}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,9 +472,10 @@
     <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +500,14 @@
       <c r="H1" t="s">
         <v>14</v>
       </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>471</v>
       </c>
@@ -511,15 +528,22 @@
         <v>8957.7627327641858</v>
       </c>
       <c r="G2" s="1">
-        <f t="shared" ref="G2:G8" si="0">C2/D2*1000000</f>
+        <f>C2/D2*1000000</f>
         <v>7342028.5570697952</v>
       </c>
       <c r="H2" s="1">
         <f>E2/D2</f>
         <v>819.62748691873355</v>
       </c>
+      <c r="I2" s="3">
+        <v>716081.2</v>
+      </c>
+      <c r="J2" s="4">
+        <f>C2/I2*1000000</f>
+        <v>346830.49911099469</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>472</v>
       </c>
@@ -536,19 +560,26 @@
         <v>3030954</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F8" si="1">C3/E3*1000000</f>
+        <f t="shared" ref="F3:F8" si="0">C3/E3*1000000</f>
         <v>7510.3086354989227</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G2:G8" si="1">C3/D3*1000000</f>
         <v>603291.63574684621</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H9" si="2">E3/D3</f>
+        <f t="shared" ref="H3:H8" si="2">E3/D3</f>
         <v>80.328474504399452</v>
       </c>
+      <c r="I3" s="3">
+        <v>94491.7</v>
+      </c>
+      <c r="J3" s="4">
+        <f>C3/I3*1000000</f>
+        <v>240903.69842007291</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>473</v>
       </c>
@@ -565,19 +596,26 @@
         <v>445857</v>
       </c>
       <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>14041.497610220316</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" si="1"/>
-        <v>14041.497610220316</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" si="0"/>
         <v>2798614.2154671433</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="2"/>
         <v>199.3102369244524</v>
       </c>
+      <c r="I4" s="5">
+        <v>12238.8</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ref="J4:J8" si="3">C4/I4*1000000</f>
+        <v>511528.90806288196</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>474</v>
       </c>
@@ -594,19 +632,27 @@
         <v>199723</v>
       </c>
       <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>14699.859305137616</v>
+      </c>
+      <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>14699.859305137616</v>
-      </c>
-      <c r="G5" s="1">
-        <f t="shared" si="0"/>
         <v>1121428.5714285714</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
         <v>76.288388082505733</v>
       </c>
+      <c r="I5">
+        <f>12917.7</f>
+        <v>12917.7</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="3"/>
+        <v>227277.3016868328</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>475</v>
       </c>
@@ -623,19 +669,26 @@
         <v>19265636</v>
       </c>
       <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>2536.0283979205251</v>
+      </c>
+      <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>2536.0283979205251</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="0"/>
         <v>1863110.1281269065</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="2"/>
         <v>734.65665039658325</v>
       </c>
+      <c r="I6" s="5">
+        <v>189021</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="3"/>
+        <v>258480.27467847485</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>476</v>
       </c>
@@ -652,19 +705,26 @@
         <v>6488737</v>
       </c>
       <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>2531.1859611508376</v>
+      </c>
+      <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>2531.1859611508376</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="0"/>
         <v>490743.39667742321</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
         <v>193.87883948846658</v>
       </c>
+      <c r="I7" s="3">
+        <v>73595.7</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="3"/>
+        <v>223167.9296480637</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>477</v>
       </c>
@@ -681,16 +741,24 @@
         <v>20946517</v>
       </c>
       <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>5087.7814196985591</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>5087.7814196985591</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="0"/>
         <v>831004.17953276576</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
         <v>163.33330994042606</v>
+      </c>
+      <c r="I8">
+        <f>383794.9</f>
+        <v>383794.9</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="3"/>
+        <v>277677.73881310044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>